<commit_message>
falta 1 ejer bp1
</commit_message>
<xml_diff>
--- a/AC/bp1/datos.xlsx
+++ b/AC/bp1/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pingu\2Info-C2\AC\bp1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAF8FBF7-9262-4257-A088-01C8796BDEF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737248FF-4252-4B93-BB6E-3A33D12DE546}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{24BEC786-FEFE-4501-AB47-44B35E2E5A4C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Nº de Componentes</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Paralelo For</t>
+  </si>
+  <si>
+    <t>ATCGRID</t>
+  </si>
+  <si>
+    <t>PC</t>
   </si>
 </sst>
 </file>
@@ -116,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -144,6 +150,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -274,7 +286,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$3:$A$15</c:f>
+              <c:f>Hoja1!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -322,7 +334,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$C$3:$C$15</c:f>
+              <c:f>Hoja1!$C$4:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -407,7 +419,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$3:$A$15</c:f>
+              <c:f>Hoja1!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -455,7 +467,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$3:$B$15</c:f>
+              <c:f>Hoja1!$B$4:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -540,7 +552,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$3:$A$15</c:f>
+              <c:f>Hoja1!$A$4:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -588,7 +600,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$D$3:$D$15</c:f>
+              <c:f>Hoja1!$D$4:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -954,7 +966,844 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>Tiempos</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES" baseline="0"/>
+              <a:t>PC</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Tiempos Secuencial</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$G$4:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33554432</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>67108864</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$H$4:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>5.4181000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0950000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.13508E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7917700000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.3927899999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.6071100000000005E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5146470000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.1952329999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0363908E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0444119E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.0421427000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.0844701000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.9852676999999997E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-CC50-4C2A-B47B-54F2826C7AA3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Tiempos For Paralelo</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$G$4:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33554432</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>67108864</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$I$4:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>7.8795489999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.299956E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7382130000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3175599999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.73754E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.7719700000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0920345E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2266948999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.1317369999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0152110000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.8423528000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.7298735E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.0856397000000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-CC50-4C2A-B47B-54F2826C7AA3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Tiempos Sections Paralelo</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$G$4:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33554432</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>67108864</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$J$4:$J$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>7.7053999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.207203E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.316088E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.1736469999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4059949999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.244081E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0935729999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.3291550000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6510990999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.4457895000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.5257149999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.2366452000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.6730505000000004E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-CC50-4C2A-B47B-54F2826C7AA3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="519052671"/>
+        <c:axId val="504385663"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="519052671"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Elementos</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES" baseline="0"/>
+                  <a:t> del vector</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="504385663"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="504385663"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Tiempo en segundos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="519052671"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1497,19 +2346,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1530,6 +2882,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1339850</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B782ADA3-8DF6-4A45-8040-2CBB46344011}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1835,10 +3223,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35F8FF4A-D33B-4B4D-80E0-8D68D7522969}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1846,216 +3234,409 @@
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="7" max="10" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="G1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
+      <c r="G2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>16384</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B4" s="2">
         <v>4.4205600000000002E-4</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C4" s="2">
         <v>1.178082E-3</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D4" s="2">
         <v>5.1984899999999996E-4</v>
       </c>
+      <c r="G4" s="1">
+        <v>16384</v>
+      </c>
+      <c r="H4" s="2">
+        <v>5.4181000000000002E-5</v>
+      </c>
+      <c r="I4" s="2">
+        <v>7.8795489999999996E-3</v>
+      </c>
+      <c r="J4" s="2">
+        <v>7.7053999999999998E-5</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>32768</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B5" s="4">
         <v>4.6292000000000002E-4</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C5" s="4">
         <v>1.191583E-3</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D5" s="4">
         <v>7.4646200000000004E-4</v>
       </c>
+      <c r="G5" s="3">
+        <v>32768</v>
+      </c>
+      <c r="H5" s="4">
+        <v>9.0950000000000002E-5</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1.299956E-2</v>
+      </c>
+      <c r="J5" s="4">
+        <v>1.207203E-3</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>65536</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B6" s="2">
         <v>5.6435100000000005E-4</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6" s="2">
         <v>4.6529400000000004E-3</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D6" s="2">
         <v>7.4566200000000002E-4</v>
       </c>
+      <c r="G6" s="1">
+        <v>65536</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2.13508E-4</v>
+      </c>
+      <c r="I6" s="2">
+        <v>3.7382130000000002E-3</v>
+      </c>
+      <c r="J6" s="2">
+        <v>4.316088E-3</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>131072</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B7" s="4">
         <v>6.7678699999999998E-4</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C7" s="4">
         <v>3.9505060000000003E-3</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D7" s="4">
         <v>2.6420910000000001E-3</v>
       </c>
+      <c r="G7" s="5">
+        <v>131072</v>
+      </c>
+      <c r="H7" s="4">
+        <v>3.7917700000000002E-4</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1.3175599999999999E-4</v>
+      </c>
+      <c r="J7" s="4">
+        <v>8.1736469999999992E-3</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>262144</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B8" s="2">
         <v>1.3812049999999999E-3</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C8" s="2">
         <v>5.0747919999999998E-3</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D8" s="2">
         <v>2.401795E-3</v>
       </c>
+      <c r="G8" s="1">
+        <v>262144</v>
+      </c>
+      <c r="H8" s="2">
+        <v>4.3927899999999999E-4</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1.73754E-4</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1.4059949999999999E-3</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>524288</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B9" s="4">
         <v>2.6722600000000001E-3</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C9" s="4">
         <v>5.8200320000000002E-3</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D9" s="4">
         <v>4.1235129999999997E-3</v>
       </c>
+      <c r="G9" s="5">
+        <v>524288</v>
+      </c>
+      <c r="H9" s="4">
+        <v>9.6071100000000005E-4</v>
+      </c>
+      <c r="I9" s="4">
+        <v>2.7719700000000002E-4</v>
+      </c>
+      <c r="J9" s="4">
+        <v>1.244081E-3</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>1048576</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
         <v>4.9931289999999998E-3</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C10" s="2">
         <v>6.058585E-3</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D10" s="2">
         <v>7.2510580000000003E-3</v>
       </c>
+      <c r="G10" s="1">
+        <v>1048576</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2.5146470000000001E-3</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1.0920345E-2</v>
+      </c>
+      <c r="J10" s="2">
+        <v>7.0935729999999997E-3</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
         <v>2097152</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B11" s="4">
         <v>9.0816089999999992E-3</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C11" s="4">
         <v>5.826052E-3</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D11" s="4">
         <v>1.3017103E-2</v>
       </c>
+      <c r="G11" s="5">
+        <v>2097152</v>
+      </c>
+      <c r="H11" s="4">
+        <v>5.1952329999999996E-3</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1.2266948999999999E-2</v>
+      </c>
+      <c r="J11" s="4">
+        <v>7.3291550000000004E-3</v>
+      </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>4194304</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B12" s="2">
         <v>1.711238E-2</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C12" s="2">
         <v>9.8222870000000007E-3</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D12" s="2">
         <v>2.5916759000000001E-2</v>
       </c>
+      <c r="G12" s="1">
+        <v>4194304</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1.0363908E-2</v>
+      </c>
+      <c r="I12" s="2">
+        <v>5.1317369999999999E-3</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1.6510990999999999E-2</v>
+      </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
         <v>8388608</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B13" s="4">
         <v>3.4459608000000003E-2</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C13" s="4">
         <v>1.6397648000000001E-2</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D13" s="4">
         <v>4.5680686999999998E-2</v>
       </c>
+      <c r="G13" s="5">
+        <v>8388608</v>
+      </c>
+      <c r="H13" s="4">
+        <v>2.0444119E-2</v>
+      </c>
+      <c r="I13" s="4">
+        <v>9.0152110000000004E-3</v>
+      </c>
+      <c r="J13" s="4">
+        <v>3.4457895000000002E-2</v>
+      </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>16777216</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B14" s="2">
         <v>6.5936852000000004E-2</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C14" s="2">
         <v>3.3309287999999999E-2</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D14" s="2">
         <v>0.105596114</v>
       </c>
+      <c r="G14" s="1">
+        <v>16777216</v>
+      </c>
+      <c r="H14" s="2">
+        <v>4.0421427000000003E-2</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1.8423528000000002E-2</v>
+      </c>
+      <c r="J14" s="2">
+        <v>5.5257149999999998E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
         <v>33554432</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B15" s="4">
         <v>0.129233605</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C15" s="4">
         <v>7.2183140000000007E-2</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D15" s="4">
         <v>0.18005073399999999</v>
       </c>
+      <c r="G15" s="5">
+        <v>33554432</v>
+      </c>
+      <c r="H15" s="4">
+        <v>8.0844701000000005E-2</v>
+      </c>
+      <c r="I15" s="4">
+        <v>3.7298735E-2</v>
+      </c>
+      <c r="J15" s="4">
+        <v>9.2366452000000002E-2</v>
+      </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
         <v>67108864</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B16" s="7">
         <v>0.12938464199999999</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C16" s="7">
         <v>7.2183140000000007E-2</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D16" s="7">
         <v>0.18005073399999999</v>
+      </c>
+      <c r="G16" s="6">
+        <v>67108864</v>
+      </c>
+      <c r="H16" s="7">
+        <v>7.9852676999999997E-2</v>
+      </c>
+      <c r="I16" s="7">
+        <v>4.0856397000000003E-2</v>
+      </c>
+      <c r="J16" s="7">
+        <v>7.6730505000000004E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
+  <mergeCells count="10">
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>